<commit_message>
Added Support for adding mulitple excel doc
</commit_message>
<xml_diff>
--- a/Lead Count API.xlsx
+++ b/Lead Count API.xlsx
@@ -31,9 +31,6 @@
     <t>Overview</t>
   </si>
   <si>
-    <t>This API is used to retrieve number of leads for an Agent.</t>
-  </si>
-  <si>
     <t>Method</t>
   </si>
   <si>
@@ -124,10 +121,13 @@
     <t>Any details of the error or message can be included in the details.</t>
   </si>
   <si>
-    <t>{ "leadCount": { "leadCount": "70" }, "systemInformation": { "errorCode": "", "errorMessage": "", "timestamp": "", "details": "" } }</t>
-  </si>
-  <si>
     <t>Response</t>
+  </si>
+  <si>
+    <t>This API is used to retrieve number of leads for an Agent. 11</t>
+  </si>
+  <si>
+    <t>{ "leadCount": { "leadCount": "11" }, "systemInformation": { "errorCode": "", "errorMessage": "", "timestamp": "", "details": "333" } }</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A1:XFD1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -501,65 +501,65 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
@@ -586,86 +586,86 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -677,18 +677,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the format based template in excel
</commit_message>
<xml_diff>
--- a/Lead Count API.xlsx
+++ b/Lead Count API.xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12893" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Lead Count API" sheetId="1" r:id="rId1"/>
+    <sheet name="Create Opportunity API" sheetId="2" r:id="rId2"/>
+    <sheet name="Update Lead API" sheetId="3" r:id="rId3"/>
+    <sheet name="Customer Listing API" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="41">
   <si>
     <t>Overview</t>
   </si>
@@ -128,6 +129,27 @@
   </si>
   <si>
     <t>{ "leadCount": { "leadCount": "11" }, "systemInformation": { "errorCode": "", "errorMessage": "", "timestamp": "", "details": "333" } }</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Col1</t>
+  </si>
+  <si>
+    <t>Col2</t>
+  </si>
+  <si>
+    <t>Col3</t>
+  </si>
+  <si>
+    <t>Col4</t>
+  </si>
+  <si>
+    <t>ResponseSample</t>
   </si>
 </sst>
 </file>
@@ -475,95 +497,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="50.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.19921875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.06640625" style="1"/>
-    <col min="7" max="7" width="29.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.19921875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="106.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.3984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.19921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -573,100 +748,262 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="56.3984375" customWidth="1"/>
+    <col min="1" max="1" width="106.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.9296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.19921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
+      <c r="C19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
+      <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="5" t="s">
+      <c r="C21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="C23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -675,21 +1012,564 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="106.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="27.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" ht="41.65" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="106.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="27.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" ht="41.65" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" ht="27.75" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" ht="27.75" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>